<commit_message>
- added L1 Autopass feature
</commit_message>
<xml_diff>
--- a/GroupStudiesTriggerStudy.xlsx
+++ b/GroupStudiesTriggerStudy.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirmuhammad/Desktop/NA62Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A670AF-6ABB-1149-881A-B7EAFD4D5343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D0E7A2-4BB2-FC4A-8B67-9F9E3EB86B12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{99C2DA6C-70A9-A943-8872-46628E1DE36A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>mu+</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>nu_mu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After LKr30 thingy </t>
   </si>
 </sst>
 </file>
@@ -228,6 +231,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -243,6 +251,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -258,6 +271,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -273,6 +291,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -288,6 +311,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -303,6 +331,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -318,6 +351,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-639A-034A-AF0C-BB1DB001BE9E}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -571,6 +609,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -586,6 +629,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -601,6 +649,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -616,6 +669,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -631,6 +689,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -646,6 +709,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -661,6 +729,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-C649-A042-A023-5E8A827D8E32}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -2002,16 +2075,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2336,10 +2409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFC9FAF3-D931-4347-A32D-034420562BFB}">
-  <dimension ref="E10:L36"/>
+  <dimension ref="E10:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2667,7 +2740,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1">
-        <f t="shared" ref="G36:L36" si="1">SUM(H29:H34)</f>
+        <f t="shared" ref="H36:K36" si="1">SUM(H29:H34)</f>
         <v>33.590000000000003</v>
       </c>
       <c r="I36" s="1">
@@ -2683,6 +2756,11 @@
         <v>5.07</v>
       </c>
       <c r="L36" s="1"/>
+    </row>
+    <row r="40" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>